<commit_message>
Added 2nd type of allocation (not in UI yet)
Removed unused files. Fixed model comparison calculations for LLF. No longer add zero point to plots if not present in data. Changed wording of tab 2 prediction label. Added comparison values back to tab 3 table.
</commit_message>
<xml_diff>
--- a/datasets/covariate_data.xlsx
+++ b/datasets/covariate_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\repos\Covariate_Tool\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F3975A-05F1-4EB0-A7EE-77165FEA8CFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA8464C-9EF6-4D16-86B9-7AEB82747BBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38292" yWindow="2580" windowWidth="17436" windowHeight="12204" activeTab="1" xr2:uid="{E306A3B3-E968-484E-9853-F350328284C5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{E306A3B3-E968-484E-9853-F350328284C5}"/>
   </bookViews>
   <sheets>
     <sheet name="DS1" sheetId="1" r:id="rId1"/>
@@ -400,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA58DA2-4B17-49DD-A384-32C5A179A21B}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,13 +414,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -431,13 +431,13 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5.3100000000000001E-2</v>
       </c>
       <c r="D2">
-        <v>5.3100000000000001E-2</v>
+        <v>4</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="C3">
+        <v>6.1899999999999997E-2</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
         <v>0</v>
-      </c>
-      <c r="D3">
-        <v>6.1899999999999997E-2</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -465,13 +465,13 @@
         <v>2</v>
       </c>
       <c r="C4">
+        <v>0.158</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>0.5</v>
-      </c>
-      <c r="D4">
-        <v>0.158</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -482,13 +482,13 @@
         <v>1</v>
       </c>
       <c r="C5">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>0.5</v>
-      </c>
-      <c r="D5">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -499,13 +499,13 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1.046</v>
       </c>
       <c r="D6">
-        <v>1.046</v>
+        <v>32</v>
       </c>
       <c r="E6">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -516,13 +516,13 @@
         <v>9</v>
       </c>
       <c r="C7">
+        <v>1.75</v>
+      </c>
+      <c r="D7">
+        <v>32</v>
+      </c>
+      <c r="E7">
         <v>5</v>
-      </c>
-      <c r="D7">
-        <v>1.75</v>
-      </c>
-      <c r="E7">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -533,13 +533,13 @@
         <v>6</v>
       </c>
       <c r="C8">
+        <v>2.96</v>
+      </c>
+      <c r="D8">
+        <v>24</v>
+      </c>
+      <c r="E8">
         <v>4.5</v>
-      </c>
-      <c r="D8">
-        <v>2.96</v>
-      </c>
-      <c r="E8">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -550,13 +550,13 @@
         <v>7</v>
       </c>
       <c r="C9">
+        <v>4.97</v>
+      </c>
+      <c r="D9">
+        <v>24</v>
+      </c>
+      <c r="E9">
         <v>2.5</v>
-      </c>
-      <c r="D9">
-        <v>4.97</v>
-      </c>
-      <c r="E9">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -567,13 +567,13 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>0.42</v>
       </c>
       <c r="D10">
-        <v>0.42</v>
+        <v>24</v>
       </c>
       <c r="E10">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -584,13 +584,13 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>4.7</v>
       </c>
       <c r="D11">
-        <v>4.7</v>
+        <v>30</v>
       </c>
       <c r="E11">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -601,10 +601,10 @@
         <v>0</v>
       </c>
       <c r="C12">
+        <v>0.9</v>
+      </c>
+      <c r="D12">
         <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0.9</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -618,13 +618,13 @@
         <v>4</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="D13">
-        <v>1.5</v>
+        <v>8</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -635,13 +635,13 @@
         <v>1</v>
       </c>
       <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
         <v>6</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14">
-        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -652,13 +652,13 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>1.2</v>
       </c>
       <c r="D15">
-        <v>1.2</v>
+        <v>12</v>
       </c>
       <c r="E15">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -669,13 +669,13 @@
         <v>2</v>
       </c>
       <c r="C16">
+        <v>1.2</v>
+      </c>
+      <c r="D16">
+        <v>20</v>
+      </c>
+      <c r="E16">
         <v>6</v>
-      </c>
-      <c r="D16">
-        <v>1.2</v>
-      </c>
-      <c r="E16">
-        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -686,13 +686,13 @@
         <v>2</v>
       </c>
       <c r="C17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D17">
+        <v>32</v>
+      </c>
+      <c r="E17">
         <v>10</v>
-      </c>
-      <c r="D17">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E17">
-        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -703,13 +703,13 @@
         <v>3</v>
       </c>
       <c r="C18">
+        <v>7.6</v>
+      </c>
+      <c r="D18">
+        <v>24</v>
+      </c>
+      <c r="E18">
         <v>8</v>
-      </c>
-      <c r="D18">
-        <v>7.6</v>
-      </c>
-      <c r="E18">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3724057A-E4DA-4229-B436-3ADE45F36CF0}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,10 +735,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -752,10 +752,10 @@
         <v>2</v>
       </c>
       <c r="C2">
+        <v>0.05</v>
+      </c>
+      <c r="D2">
         <v>1.3</v>
-      </c>
-      <c r="D2">
-        <v>0.05</v>
       </c>
       <c r="E2">
         <v>0.5</v>
@@ -769,10 +769,10 @@
         <v>11</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>17.8</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
       </c>
       <c r="E3">
         <v>2.8</v>
@@ -786,10 +786,10 @@
         <v>2</v>
       </c>
       <c r="C4">
+        <v>0.19</v>
+      </c>
+      <c r="D4">
         <v>5</v>
-      </c>
-      <c r="D4">
-        <v>0.19</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -803,10 +803,10 @@
         <v>4</v>
       </c>
       <c r="C5">
+        <v>0.41</v>
+      </c>
+      <c r="D5">
         <v>1.5</v>
-      </c>
-      <c r="D5">
-        <v>0.41</v>
       </c>
       <c r="E5">
         <v>0.5</v>
@@ -820,10 +820,10 @@
         <v>3</v>
       </c>
       <c r="C6">
+        <v>0.32</v>
+      </c>
+      <c r="D6">
         <v>1.5</v>
-      </c>
-      <c r="D6">
-        <v>0.32</v>
       </c>
       <c r="E6">
         <v>0.5</v>
@@ -837,10 +837,10 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>0.61</v>
       </c>
       <c r="D7">
-        <v>0.61</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -854,10 +854,10 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>0.32</v>
       </c>
       <c r="D8">
-        <v>0.32</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>0.5</v>
@@ -871,10 +871,10 @@
         <v>2</v>
       </c>
       <c r="C9">
+        <v>1.83</v>
+      </c>
+      <c r="D9">
         <v>8</v>
-      </c>
-      <c r="D9">
-        <v>1.83</v>
       </c>
       <c r="E9">
         <v>2.5</v>
@@ -888,10 +888,10 @@
         <v>4</v>
       </c>
       <c r="C10">
+        <v>3.01</v>
+      </c>
+      <c r="D10">
         <v>30</v>
-      </c>
-      <c r="D10">
-        <v>3.01</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -905,10 +905,10 @@
         <v>0</v>
       </c>
       <c r="C11">
+        <v>1.79</v>
+      </c>
+      <c r="D11">
         <v>9</v>
-      </c>
-      <c r="D11">
-        <v>1.79</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -922,10 +922,10 @@
         <v>4</v>
       </c>
       <c r="C12">
+        <v>3.17</v>
+      </c>
+      <c r="D12">
         <v>25</v>
-      </c>
-      <c r="D12">
-        <v>3.17</v>
       </c>
       <c r="E12">
         <v>6</v>
@@ -939,10 +939,10 @@
         <v>1</v>
       </c>
       <c r="C13">
+        <v>3.4</v>
+      </c>
+      <c r="D13">
         <v>15</v>
-      </c>
-      <c r="D13">
-        <v>3.4</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -956,10 +956,10 @@
         <v>3</v>
       </c>
       <c r="C14">
+        <v>4.2</v>
+      </c>
+      <c r="D14">
         <v>15</v>
-      </c>
-      <c r="D14">
-        <v>4.2</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -973,10 +973,10 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="D15">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="E15">
         <v>1</v>

</xml_diff>

<commit_message>
Can subset imported data, sort results table columns
mvfList of Model class changed to mvf_array. Failure intensity prediction performed by iterating over intervals and checking if intensity is less than specified value; currently just prints to console.
</commit_message>
<xml_diff>
--- a/datasets/covariate_data.xlsx
+++ b/datasets/covariate_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\repos\Covariate_Tool\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA8464C-9EF6-4D16-86B9-7AEB82747BBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F324C3EE-ABED-4A55-B39D-F8CA37BA6DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{E306A3B3-E968-484E-9853-F350328284C5}"/>
+    <workbookView xWindow="43536" yWindow="2412" windowWidth="17436" windowHeight="12204" xr2:uid="{E306A3B3-E968-484E-9853-F350328284C5}"/>
   </bookViews>
   <sheets>
     <sheet name="DS1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>